<commit_message>
Translated guide reshape to en
</commit_message>
<xml_diff>
--- a/administration/Sammanställning april 2021.xlsx
+++ b/administration/Sammanställning april 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xsunde/Dropbox/Jupyter/stathelp/administration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB552397-30B3-F642-8027-FAD921A33F67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CB1A06-2F72-F34F-B94C-17FC2007E4E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3960" yWindow="940" windowWidth="16460" windowHeight="15400" xr2:uid="{558F00F3-C016-DA44-9344-CE8B64536B3C}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>https://www.stathelp.se/sv/histogram_sv.html</t>
   </si>
   <si>
-    <t>https://www.stathelp.se/sv/ifstatements_sv.html</t>
-  </si>
-  <si>
     <t>https://www.stathelp.se/sv/linecharts_sv.html</t>
   </si>
   <si>
@@ -268,6 +265,9 @@
   </si>
   <si>
     <t>https://www.stathelp.se/sv/regression_interaction2_en.html</t>
+  </si>
+  <si>
+    <t>(ifstatements_sv.html)</t>
   </si>
 </sst>
 </file>
@@ -621,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C3E5DE-A269-4247-953D-AAEB8ADEAD60}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -633,69 +633,69 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
         <v>76</v>
-      </c>
-      <c r="B1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>739</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>45</v>
+        <v>178</v>
       </c>
       <c r="C3">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>165</v>
       </c>
       <c r="C4">
-        <v>317</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>152</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
         <v>68</v>
@@ -703,13 +703,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>178</v>
+        <v>145</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>45</v>
@@ -717,140 +717,158 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B7">
-        <v>55</v>
-      </c>
-      <c r="C7">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>60</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B8">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B9">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B10">
-        <v>40</v>
-      </c>
-      <c r="C10">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B11">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="C11">
-        <v>175</v>
+        <v>2968</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B12">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="C12">
-        <v>137</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>79</v>
+      </c>
+      <c r="C13">
+        <v>194</v>
+      </c>
+      <c r="D13" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>78</v>
+      </c>
+      <c r="C14">
+        <v>73</v>
+      </c>
+      <c r="D14" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>90</v>
+        <v>72</v>
+      </c>
+      <c r="C15">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>69</v>
+      </c>
+      <c r="C16">
+        <v>175</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="C17">
+        <v>118</v>
+      </c>
+      <c r="D17" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B18">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="C18">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -864,82 +882,91 @@
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B20">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="C20">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="B21">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C21">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B22">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C22">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B23">
-        <v>165</v>
+        <v>38</v>
       </c>
       <c r="C23">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>37</v>
+      </c>
+      <c r="C24">
+        <v>137</v>
+      </c>
+      <c r="D24" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B25">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="C25">
-        <v>118</v>
+        <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -947,130 +974,124 @@
         <v>35</v>
       </c>
       <c r="B26">
-        <v>38</v>
-      </c>
-      <c r="C26">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B27">
-        <v>18</v>
+        <v>31</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="B28">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C28">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="B29">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="C29">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="B30">
-        <v>152</v>
+        <v>28</v>
       </c>
       <c r="C30">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B31">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="C31">
-        <v>2968</v>
+        <v>45</v>
       </c>
       <c r="D31" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B32">
-        <v>84</v>
-      </c>
-      <c r="C32">
-        <v>31</v>
-      </c>
-      <c r="D32" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B33">
-        <v>12</v>
-      </c>
-      <c r="D33" t="s">
-        <v>80</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="B34">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="C34">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B35">
-        <v>119</v>
+        <v>15</v>
       </c>
       <c r="C35">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1078,117 +1099,96 @@
         <v>33</v>
       </c>
       <c r="B36">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B37">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="C37">
-        <v>73</v>
+        <v>279</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B38">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="D38" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B39">
-        <v>136</v>
+        <v>7</v>
+      </c>
+      <c r="C39">
+        <v>317</v>
+      </c>
+      <c r="D39" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B40">
-        <v>12</v>
-      </c>
-      <c r="C40">
-        <v>279</v>
-      </c>
-      <c r="D40" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B41">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B42">
-        <v>35</v>
-      </c>
-      <c r="D42" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B43">
-        <v>739</v>
-      </c>
-      <c r="C43">
-        <v>7</v>
-      </c>
-      <c r="D43" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B44">
-        <v>123</v>
-      </c>
-      <c r="C44">
-        <v>7</v>
-      </c>
-      <c r="D44" t="s">
-        <v>58</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>39</v>
-      </c>
-      <c r="B45">
-        <v>79</v>
-      </c>
-      <c r="C45">
-        <v>194</v>
-      </c>
-      <c r="D45" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:D33">
-    <sortCondition ref="D2:D33"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D45">
+    <sortCondition descending="1" ref="B2:B45"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>